<commit_message>
fixed issues on market shares and total output in activities added to clusters of regions
</commit_message>
<xml_diff>
--- a/master.xlsx
+++ b/master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lorenzorinaldi/Documents/GitHub/SESAM/IAM-COMPACT-Study-8/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F9B643D-23FE-6445-8DBE-85BC556A3531}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BCC8EC0-15F0-6342-A4BA-393616C84782}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-9240" yWindow="-28300" windowWidth="25600" windowHeight="26880" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Master" sheetId="1" r:id="rId1"/>
@@ -2849,8 +2849,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView zoomScale="200" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3289,8 +3289,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView zoomScale="200" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>